<commit_message>
getting close to done!
</commit_message>
<xml_diff>
--- a/SelectionPerformance.xlsx
+++ b/SelectionPerformance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoff/Documents/MyDocuments/Research/ATP General/AxiomSelectionEvaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376E235-5CEE-8F41-BE1C-410DC385FEE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA587CC3-BC17-534C-8F92-8999065BB17F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28180" yWindow="480" windowWidth="24880" windowHeight="15540" xr2:uid="{B36EBB89-D31F-064D-885A-C818348F52FE}"/>
+    <workbookView xWindow="-24920" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{B36EBB89-D31F-064D-885A-C818348F52FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,10 +1010,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>0.37</v>
+        <v>0.36087121474350697</v>
       </c>
       <c r="D9" s="3">
-        <v>0.77</v>
+        <v>0.56937035610904596</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -1022,25 +1022,25 @@
         <v>9</v>
       </c>
       <c r="G9" s="2">
-        <v>315</v>
+        <v>235</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>0.96923076923076923</v>
+        <v>0.72307692307692306</v>
       </c>
       <c r="I9" s="1">
-        <v>0.38</v>
+        <v>0.49907721187931903</v>
       </c>
       <c r="J9" s="3">
-        <v>0.8</v>
+        <v>0.61139622805221505</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1">
-        <v>0.05</v>
+        <v>4.9124916365531297E-2</v>
       </c>
       <c r="N9" s="3">
-        <v>0.93</v>
+        <v>0.79065971708551697</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>9</v>
@@ -1049,17 +1049,17 @@
         <v>9</v>
       </c>
       <c r="Q9" s="2">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="R9" s="3">
         <f t="shared" si="1"/>
-        <v>0.96307692307692305</v>
+        <v>0.85538461538461541</v>
       </c>
       <c r="S9" s="1">
-        <v>0.05</v>
+        <v>5.7430207981286598E-2</v>
       </c>
       <c r="T9" s="3">
-        <v>0.96</v>
+        <v>0.85263306574424202</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>9</v>
@@ -1712,10 +1712,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>0.21156901420760299</v>
+        <v>0.205770491432575</v>
       </c>
       <c r="D24" s="3">
-        <v>0.693570566224605</v>
+        <v>0.693555671227017</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>9</v>
@@ -1724,17 +1724,17 @@
         <v>9</v>
       </c>
       <c r="G24" s="2">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="3"/>
-        <v>0.5828497743391361</v>
+        <v>0.58027079303675044</v>
       </c>
       <c r="I24" s="1">
-        <v>0.36299064273893</v>
+        <v>0.35461114690213802</v>
       </c>
       <c r="J24" s="3">
-        <v>0.756973451437985</v>
+        <v>0.75805200671086503</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>9</v>
@@ -1743,10 +1743,10 @@
         <v>9</v>
       </c>
       <c r="M24" s="6">
-        <v>3.4628953280996001E-2</v>
+        <v>3.4127416057395797E-2</v>
       </c>
       <c r="N24" s="3">
-        <v>0.39881229987260203</v>
+        <v>0.399974400676194</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>9</v>
@@ -1755,17 +1755,17 @@
         <v>9</v>
       </c>
       <c r="Q24" s="2">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="R24" s="3">
         <f t="shared" si="4"/>
-        <v>0.87099125364431484</v>
+        <v>0.86807580174927113</v>
       </c>
       <c r="S24" s="6">
-        <v>3.9758095315084903E-2</v>
+        <v>3.92279030920024E-2</v>
       </c>
       <c r="T24" s="3">
-        <v>0.41137784234260599</v>
+        <v>0.41294973356557202</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>9</v>
@@ -1782,66 +1782,66 @@
         <v>19</v>
       </c>
       <c r="C25" s="1">
-        <v>0.33127747108372402</v>
+        <v>0.32603692591421801</v>
       </c>
       <c r="D25" s="3">
-        <v>0.54027346115695696</v>
+        <v>0.540485768850547</v>
       </c>
       <c r="E25" s="1">
-        <v>0.55277880108107902</v>
+        <v>0.54928383533993297</v>
       </c>
       <c r="F25" s="1">
-        <v>0.41681233053711803</v>
+        <v>0.41310262328491898</v>
       </c>
       <c r="G25" s="2">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="3"/>
-        <v>0.68536428110896197</v>
+        <v>0.6840747904577692</v>
       </c>
       <c r="I25" s="1">
-        <v>0.48335969675527402</v>
+        <v>0.476610058523047</v>
       </c>
       <c r="J25" s="3">
-        <v>0.59071618655960101</v>
+        <v>0.59136620874102797</v>
       </c>
       <c r="K25" s="1">
-        <v>0.80654743224530001</v>
+        <v>0.802958745157622</v>
       </c>
       <c r="L25" s="1">
-        <v>0.60816173533684903</v>
+        <v>0.60388517315260104</v>
       </c>
       <c r="M25" s="6">
-        <v>2.9728901814692999E-2</v>
+        <v>2.8778568657515199E-2</v>
       </c>
       <c r="N25" s="3">
-        <v>0.53276753731375603</v>
+        <v>0.53279319371673095</v>
       </c>
       <c r="O25" s="1">
-        <v>0.46451371646047102</v>
+        <v>0.45623229977916302</v>
       </c>
       <c r="P25" s="1">
-        <v>6.7746215026233694E-2</v>
+        <v>7.20734073534815E-2</v>
       </c>
       <c r="Q25" s="2">
-        <v>1140</v>
+        <v>1115</v>
       </c>
       <c r="R25" s="3">
         <f t="shared" si="4"/>
-        <v>0.83090379008746351</v>
+        <v>0.81268221574344024</v>
       </c>
       <c r="S25" s="6">
-        <v>3.5778994113823501E-2</v>
+        <v>3.5334404028823603E-2</v>
       </c>
       <c r="T25" s="3">
-        <v>0.56052119504651499</v>
+        <v>0.55892886314922097</v>
       </c>
       <c r="U25" s="1">
-        <v>0.55904633244190005</v>
+        <v>0.56016324519970795</v>
       </c>
       <c r="V25" s="1">
-        <v>8.15331640491163E-2</v>
+        <v>8.8491923468086306E-2</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>